<commit_message>
Add latest timesheets, update backend and frontend code
</commit_message>
<xml_diff>
--- a/backend/storage/timesheet_14_2025-10-13.xlsx
+++ b/backend/storage/timesheet_14_2025-10-13.xlsx
@@ -469,8 +469,10 @@
           <t>Jose Flores</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -520,16 +522,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>363</t>
+          <t>712</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Box Truck</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
+          <t>Paver</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>

</xml_diff>